<commit_message>
Added Light, Heavy, and Average traffic policies to VerticalRoad
</commit_message>
<xml_diff>
--- a/Spreadsheet with simulation information.xlsx
+++ b/Spreadsheet with simulation information.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92c614ef88483475/Documents/Pitt2022/CS1980/team-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connp\OneDrive\Documents\_Pitt\Traffic_Capstone\team-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{4473A5AD-1EF3-4BC0-9281-A8B0B0E8898C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C178548-320E-4A40-93BD-E683496A65CB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649A0C4F-8987-4F1D-A3C7-2D36F1061F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4259BDF6-7017-4B3A-89CE-363379D156E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4259BDF6-7017-4B3A-89CE-363379D156E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -214,9 +213,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$B$2</c:f>
+              <c:f>Sheet1!$B$1:$B$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Green Corridor</c:v>
                 </c:pt>
@@ -238,14 +237,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                    <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -262,31 +261,49 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -296,14 +313,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$3:$B$35</c15:sqref>
+                    <c15:sqref>Sheet1!$B$2:$B$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$3:$B$7,Sheet1!$B$9:$B$10,Sheet1!$B$13:$B$17,Sheet1!$B$20:$B$21)</c:f>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>51</c:v>
                 </c:pt>
@@ -320,31 +337,49 @@
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>69</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,9 +395,9 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$D$2</c:f>
+              <c:f>Sheet1!$D$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Red Freeze</c:v>
                 </c:pt>
@@ -384,14 +419,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                    <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -408,31 +443,49 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -442,14 +495,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$D$3:$D$35</c15:sqref>
+                    <c15:sqref>Sheet1!$D$2:$D$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$D$3:$D$7,Sheet1!$D$9:$D$10,Sheet1!$D$13:$D$17,Sheet1!$D$20:$D$21)</c:f>
+              <c:f>Sheet1!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>54</c:v>
                 </c:pt>
@@ -466,31 +519,49 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,9 +577,9 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1:$F$2</c:f>
+              <c:f>Sheet1!$F$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Control</c:v>
                 </c:pt>
@@ -530,14 +601,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                    <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -554,31 +625,49 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,14 +677,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$F$3:$F$35</c15:sqref>
+                    <c15:sqref>Sheet1!$F$2:$F$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$F$3:$F$7,Sheet1!$F$9:$F$10,Sheet1!$F$13:$F$17,Sheet1!$F$20:$F$21)</c:f>
+              <c:f>Sheet1!$F$2:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -612,31 +701,49 @@
                   <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>94</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,15 +777,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$1:$C$2</c15:sqref>
+                          <c15:sqref>Sheet1!$C$1:$C$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>Green Corridor</c:v>
-                      </c:pt>
+                      <c:ptCount val="1"/>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
@@ -697,16 +801,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -723,31 +827,49 @@
                         <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>7</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>12</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>13</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>14</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>15</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>18</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -757,16 +879,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$C$3:$C$35</c15:sqref>
+                          <c15:sqref>Sheet1!$C$2:$C$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$C$3:$C$7,Sheet1!$C$9:$C$10,Sheet1!$C$13:$C$17,Sheet1!$C$20:$C$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$C$2:$C$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>3980</c:v>
                       </c:pt>
@@ -783,31 +905,49 @@
                         <c:v>833</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>723</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>626</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>551</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>8335</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>7424</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>395</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>386</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>374</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>374</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>339</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>4106</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>4377</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>294</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>281</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>4052</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -828,15 +968,12 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$1:$E$2</c15:sqref>
+                          <c15:sqref>Sheet1!$E$1:$E$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>Red Freeze</c:v>
-                      </c:pt>
+                      <c:ptCount val="1"/>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
@@ -855,16 +992,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -881,31 +1018,49 @@
                         <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>7</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>12</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>13</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>14</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>15</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>18</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -915,16 +1070,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$E$3:$E$35</c15:sqref>
+                          <c15:sqref>Sheet1!$E$2:$E$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$E$3:$E$7,Sheet1!$E$9:$E$10,Sheet1!$E$13:$E$17,Sheet1!$E$20:$E$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$E$2:$E$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>4072</c:v>
                       </c:pt>
@@ -941,31 +1096,49 @@
                         <c:v>929</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>9562</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>647</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>587</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>499</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>417</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>445</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>402</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>401</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>385</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>348</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>359</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>295</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>294</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>295</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>260</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -986,15 +1159,12 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$G$1:$G$2</c15:sqref>
+                          <c15:sqref>Sheet1!$G$1:$G$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>Control</c:v>
-                      </c:pt>
+                      <c:ptCount val="1"/>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
@@ -1013,16 +1183,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1039,31 +1209,49 @@
                         <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>7</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>12</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>13</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>14</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>15</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>18</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1073,16 +1261,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$G$3:$G$35</c15:sqref>
+                          <c15:sqref>Sheet1!$G$2:$G$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$G$3:$G$7,Sheet1!$G$9:$G$10,Sheet1!$G$13:$G$17,Sheet1!$G$20:$G$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$G$2:$G$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>4096</c:v>
                       </c:pt>
@@ -1099,31 +1287,49 @@
                         <c:v>865</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>713</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>657</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>604</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>508</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>428</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>507</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>406</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>380</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>385</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>318</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>323</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>303</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>292</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>301</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>3149</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1527,12 +1733,9 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$C$2</c:f>
+              <c:f>Sheet1!$C$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Green Corridor</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1551,14 +1754,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                    <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1575,31 +1778,49 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,14 +1830,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$C$3:$C$35</c15:sqref>
+                    <c15:sqref>Sheet1!$C$2:$C$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$C$3:$C$7,Sheet1!$C$9:$C$10,Sheet1!$C$13:$C$17,Sheet1!$C$20:$C$21)</c:f>
+              <c:f>Sheet1!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3980</c:v>
                 </c:pt>
@@ -1633,31 +1854,49 @@
                   <c:v>833</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>626</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>551</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>8335</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7424</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>386</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>374</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>374</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>339</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>4106</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4377</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>294</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1673,12 +1912,9 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1:$E$2</c:f>
+              <c:f>Sheet1!$E$1:$E$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Red Freeze</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1697,14 +1933,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                    <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1721,31 +1957,49 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1755,14 +2009,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$E$3:$E$35</c15:sqref>
+                    <c15:sqref>Sheet1!$E$2:$E$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$E$3:$E$7,Sheet1!$E$9:$E$10,Sheet1!$E$13:$E$17,Sheet1!$E$20:$E$21)</c:f>
+              <c:f>Sheet1!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>4072</c:v>
                 </c:pt>
@@ -1779,31 +2033,49 @@
                   <c:v>929</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>9562</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>647</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>587</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>445</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>402</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>401</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>385</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>294</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1819,12 +2091,9 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1:$G$2</c:f>
+              <c:f>Sheet1!$G$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Control</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1843,14 +2112,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                    <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1867,31 +2136,49 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1901,14 +2188,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$G$3:$G$35</c15:sqref>
+                    <c15:sqref>Sheet1!$G$2:$G$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$G$3:$G$7,Sheet1!$G$9:$G$10,Sheet1!$G$13:$G$17,Sheet1!$G$20:$G$21)</c:f>
+              <c:f>Sheet1!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>4096</c:v>
                 </c:pt>
@@ -1925,31 +2212,49 @@
                   <c:v>865</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>604</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>507</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>380</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>385</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>318</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>292</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1983,12 +2288,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1:$B$2</c15:sqref>
+                          <c15:sqref>Sheet1!$B$1:$B$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="1"/>
                       <c:pt idx="0">
                         <c:v>Green Corridor</c:v>
                       </c:pt>
@@ -2010,16 +2315,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -2036,31 +2341,49 @@
                         <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>7</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>12</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>13</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>14</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>15</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>18</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2070,16 +2393,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$B$3:$B$35</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$B$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$B$3:$B$7,Sheet1!$B$9:$B$10,Sheet1!$B$13:$B$17,Sheet1!$B$20:$B$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$B$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>51</c:v>
                       </c:pt>
@@ -2096,31 +2419,49 @@
                         <c:v>56</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>55</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>62</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>70</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
                         <c:v>67</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="9">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
                         <c:v>69</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>71</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>49</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>51</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>57</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>60</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>67</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2141,12 +2482,12 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$1:$D$2</c15:sqref>
+                          <c15:sqref>Sheet1!$D$1:$D$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="1"/>
                       <c:pt idx="0">
                         <c:v>Red Freeze</c:v>
                       </c:pt>
@@ -2168,16 +2509,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -2194,31 +2535,49 @@
                         <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>7</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>12</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>13</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>14</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>15</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>18</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2228,16 +2587,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$D$3:$D$35</c15:sqref>
+                          <c15:sqref>Sheet1!$D$2:$D$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$D$3:$D$7,Sheet1!$D$9:$D$10,Sheet1!$D$13:$D$17,Sheet1!$D$20:$D$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$D$2:$D$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>54</c:v>
                       </c:pt>
@@ -2254,31 +2613,49 @@
                         <c:v>63</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>93</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>62</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>67</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>57</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>64</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>62</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>54</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>58</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>57</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>51</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2299,12 +2676,12 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1:$F$2</c15:sqref>
+                          <c15:sqref>Sheet1!$F$1:$F$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="1"/>
                       <c:pt idx="0">
                         <c:v>Control</c:v>
                       </c:pt>
@@ -2326,16 +2703,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$3:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$3:$A$7,Sheet1!$A$9:$A$10,Sheet1!$A$13:$A$17,Sheet1!$A$20:$A$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -2352,31 +2729,49 @@
                         <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>7</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>11</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>12</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>13</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>14</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>15</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>18</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2386,16 +2781,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$F$3:$F$35</c15:sqref>
+                          <c15:sqref>Sheet1!$F$2:$F$34</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$F$3:$F$7,Sheet1!$F$9:$F$10,Sheet1!$F$13:$F$17,Sheet1!$F$20:$F$21)</c15:sqref>
+                          <c15:sqref>Sheet1!$F$2:$F$21</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>84</c:v>
                       </c:pt>
@@ -2412,31 +2807,49 @@
                         <c:v>174</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
                         <c:v>94</c:v>
                       </c:pt>
-                      <c:pt idx="6">
+                      <c:pt idx="7">
                         <c:v>83</c:v>
                       </c:pt>
-                      <c:pt idx="7">
+                      <c:pt idx="8">
+                        <c:v>79</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>80</c:v>
                       </c:pt>
-                      <c:pt idx="8">
+                      <c:pt idx="11">
                         <c:v>70</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="12">
                         <c:v>77</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="13">
                         <c:v>95</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="14">
                         <c:v>88</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="15">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>79</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
                         <c:v>74</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="18">
                         <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>91</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3845,14 +4258,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>145342</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>138907</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>49610</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>257968</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>76643</xdr:rowOff>
+      <xdr:rowOff>165940</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3916,10 +4329,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4219,24 +4628,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDC7A1F-594B-4F6A-AA70-42FD9DBE002B}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="32" zoomScaleNormal="32" workbookViewId="0">
-      <selection activeCell="BO26" sqref="BO26"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
-    <col min="5" max="5" width="25.1796875" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4250,468 +4662,463 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>3980</v>
+      </c>
+      <c r="D2">
+        <v>54</v>
+      </c>
+      <c r="E2">
+        <v>4072</v>
+      </c>
+      <c r="F2">
+        <v>84</v>
+      </c>
+      <c r="G2">
+        <v>4096</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <v>2030</v>
+      </c>
+      <c r="D3">
+        <v>73</v>
+      </c>
+      <c r="E3">
+        <v>2117</v>
+      </c>
+      <c r="F3">
+        <v>109</v>
+      </c>
+      <c r="G3">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>51</v>
       </c>
-      <c r="C3">
-        <v>3980</v>
-      </c>
-      <c r="D3">
-        <v>54</v>
-      </c>
-      <c r="E3">
-        <v>4072</v>
-      </c>
-      <c r="F3">
-        <v>84</v>
-      </c>
-      <c r="G3">
-        <v>4096</v>
+      <c r="C4">
+        <v>1364</v>
+      </c>
+      <c r="D4">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>1371</v>
+      </c>
+      <c r="F4">
+        <v>72</v>
+      </c>
+      <c r="G4">
+        <v>1378</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>76</v>
-      </c>
-      <c r="C4">
-        <v>2030</v>
-      </c>
-      <c r="D4">
-        <v>73</v>
-      </c>
-      <c r="E4">
-        <v>2117</v>
-      </c>
-      <c r="F4">
-        <v>109</v>
-      </c>
-      <c r="G4">
-        <v>2056</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>1060</v>
+      </c>
+      <c r="D5">
+        <v>69</v>
+      </c>
+      <c r="E5">
+        <v>1105</v>
+      </c>
+      <c r="F5">
+        <v>130</v>
+      </c>
+      <c r="G5">
+        <v>1031</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>51</v>
-      </c>
-      <c r="C5">
-        <v>1364</v>
-      </c>
-      <c r="D5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>833</v>
+      </c>
+      <c r="D6">
+        <v>63</v>
+      </c>
+      <c r="E6">
+        <v>929</v>
+      </c>
+      <c r="F6">
+        <v>174</v>
+      </c>
+      <c r="G6">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>723</v>
+      </c>
+      <c r="D7">
+        <v>93</v>
+      </c>
+      <c r="E7">
+        <v>9562</v>
+      </c>
+      <c r="F7">
+        <v>53</v>
+      </c>
+      <c r="G7">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>62</v>
       </c>
-      <c r="E5">
-        <v>1371</v>
-      </c>
-      <c r="F5">
+      <c r="C8">
+        <v>626</v>
+      </c>
+      <c r="D8">
+        <v>62</v>
+      </c>
+      <c r="E8">
+        <v>647</v>
+      </c>
+      <c r="F8">
+        <v>94</v>
+      </c>
+      <c r="G8">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>551</v>
+      </c>
+      <c r="D9">
+        <v>67</v>
+      </c>
+      <c r="E9">
+        <v>587</v>
+      </c>
+      <c r="F9">
+        <v>83</v>
+      </c>
+      <c r="G9">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>8335</v>
+      </c>
+      <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <v>499</v>
+      </c>
+      <c r="F10">
+        <v>79</v>
+      </c>
+      <c r="G10">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>72</v>
       </c>
-      <c r="G5">
-        <v>1378</v>
+      <c r="C11">
+        <v>7424</v>
+      </c>
+      <c r="D11">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>417</v>
+      </c>
+      <c r="F11">
+        <v>85</v>
+      </c>
+      <c r="G11">
+        <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>67</v>
+      </c>
+      <c r="C12">
+        <v>395</v>
+      </c>
+      <c r="D12">
+        <v>57</v>
+      </c>
+      <c r="E12">
+        <v>445</v>
+      </c>
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="G12">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>69</v>
       </c>
-      <c r="C6">
-        <v>1060</v>
-      </c>
-      <c r="D6">
-        <v>69</v>
-      </c>
-      <c r="E6">
-        <v>1105</v>
-      </c>
-      <c r="F6">
-        <v>130</v>
-      </c>
-      <c r="G6">
-        <v>1031</v>
+      <c r="C13">
+        <v>386</v>
+      </c>
+      <c r="D13">
+        <v>64</v>
+      </c>
+      <c r="E13">
+        <v>402</v>
+      </c>
+      <c r="F13">
+        <v>70</v>
+      </c>
+      <c r="G13">
+        <v>406</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>56</v>
-      </c>
-      <c r="C7">
-        <v>833</v>
-      </c>
-      <c r="D7">
-        <v>63</v>
-      </c>
-      <c r="E7">
-        <v>929</v>
-      </c>
-      <c r="F7">
-        <v>174</v>
-      </c>
-      <c r="G7">
-        <v>865</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>71</v>
+      </c>
+      <c r="C14">
+        <v>374</v>
+      </c>
+      <c r="D14">
+        <v>62</v>
+      </c>
+      <c r="E14">
+        <v>401</v>
+      </c>
+      <c r="F14">
+        <v>77</v>
+      </c>
+      <c r="G14">
+        <v>380</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>62</v>
-      </c>
-      <c r="C9">
-        <v>626</v>
-      </c>
-      <c r="D9">
-        <v>62</v>
-      </c>
-      <c r="E9">
-        <v>647</v>
-      </c>
-      <c r="F9">
-        <v>94</v>
-      </c>
-      <c r="G9">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>70</v>
-      </c>
-      <c r="C10">
-        <v>551</v>
-      </c>
-      <c r="D10">
-        <v>67</v>
-      </c>
-      <c r="E10">
-        <v>587</v>
-      </c>
-      <c r="F10">
-        <v>83</v>
-      </c>
-      <c r="G10">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>67</v>
-      </c>
-      <c r="C13">
-        <v>395</v>
-      </c>
-      <c r="D13">
-        <v>57</v>
-      </c>
-      <c r="E13">
-        <v>445</v>
-      </c>
-      <c r="F13">
-        <v>80</v>
-      </c>
-      <c r="G13">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>69</v>
-      </c>
-      <c r="C14">
-        <v>386</v>
-      </c>
-      <c r="D14">
-        <v>64</v>
-      </c>
-      <c r="E14">
-        <v>402</v>
-      </c>
-      <c r="F14">
-        <v>70</v>
-      </c>
-      <c r="G14">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>374</v>
       </c>
       <c r="D15">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E15">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="F15">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="G15">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16">
-        <v>374</v>
+        <v>339</v>
       </c>
       <c r="D16">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E16">
-        <v>385</v>
+        <v>348</v>
       </c>
       <c r="F16">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G16">
-        <v>385</v>
+        <v>318</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
+        <v>71</v>
+      </c>
+      <c r="C17">
+        <v>4106</v>
+      </c>
+      <c r="D17">
+        <v>66</v>
+      </c>
+      <c r="E17">
+        <v>359</v>
+      </c>
+      <c r="F17">
+        <v>71</v>
+      </c>
+      <c r="G17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>57</v>
+      </c>
+      <c r="C18">
+        <v>4377</v>
+      </c>
+      <c r="D18">
+        <v>63</v>
+      </c>
+      <c r="E18">
+        <v>295</v>
+      </c>
+      <c r="F18">
+        <v>79</v>
+      </c>
+      <c r="G18">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>294</v>
+      </c>
+      <c r="D19">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>294</v>
+      </c>
+      <c r="F19">
+        <v>74</v>
+      </c>
+      <c r="G19">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>281</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
+      </c>
+      <c r="E20">
+        <v>295</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>67</v>
+      </c>
+      <c r="C21">
+        <v>4052</v>
+      </c>
+      <c r="D21">
         <v>51</v>
       </c>
-      <c r="C17">
-        <v>339</v>
-      </c>
-      <c r="D17">
-        <v>58</v>
-      </c>
-      <c r="E17">
-        <v>348</v>
-      </c>
-      <c r="F17">
-        <v>88</v>
-      </c>
-      <c r="G17">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>60</v>
-      </c>
-      <c r="C20">
-        <v>294</v>
-      </c>
-      <c r="D20">
-        <v>57</v>
-      </c>
-      <c r="E20">
-        <v>294</v>
-      </c>
-      <c r="F20">
-        <v>74</v>
-      </c>
-      <c r="G20">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>50</v>
-      </c>
-      <c r="C21">
-        <v>281</v>
-      </c>
-      <c r="D21">
-        <v>45</v>
-      </c>
       <c r="E21">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="F21">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="G21">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>6</v>
-      </c>
-      <c r="B30">
-        <v>55</v>
-      </c>
-      <c r="C30">
-        <v>723</v>
-      </c>
-      <c r="D30">
-        <v>93</v>
-      </c>
-      <c r="E30">
-        <v>9562</v>
-      </c>
-      <c r="F30">
-        <v>53</v>
-      </c>
-      <c r="G30">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>9</v>
-      </c>
-      <c r="B31">
-        <v>67</v>
-      </c>
-      <c r="C31">
-        <v>8335</v>
-      </c>
-      <c r="D31">
-        <v>70</v>
-      </c>
-      <c r="E31">
-        <v>499</v>
-      </c>
-      <c r="F31">
-        <v>79</v>
-      </c>
-      <c r="G31">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>10</v>
-      </c>
-      <c r="B32">
-        <v>72</v>
-      </c>
-      <c r="C32">
-        <v>7424</v>
-      </c>
-      <c r="D32">
-        <v>69</v>
-      </c>
-      <c r="E32">
-        <v>417</v>
-      </c>
-      <c r="F32">
-        <v>85</v>
-      </c>
-      <c r="G32">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>16</v>
-      </c>
-      <c r="B33">
-        <v>71</v>
-      </c>
-      <c r="C33">
-        <v>4106</v>
-      </c>
-      <c r="D33">
-        <v>66</v>
-      </c>
-      <c r="E33">
-        <v>359</v>
-      </c>
-      <c r="F33">
-        <v>71</v>
-      </c>
-      <c r="G33">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>17</v>
-      </c>
-      <c r="B34">
-        <v>57</v>
-      </c>
-      <c r="C34">
-        <v>4377</v>
-      </c>
-      <c r="D34">
-        <v>63</v>
-      </c>
-      <c r="E34">
-        <v>295</v>
-      </c>
-      <c r="F34">
-        <v>79</v>
-      </c>
-      <c r="G34">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>20</v>
-      </c>
-      <c r="B35">
-        <v>67</v>
-      </c>
-      <c r="C35">
-        <v>4052</v>
-      </c>
-      <c r="D35">
-        <v>51</v>
-      </c>
-      <c r="E35">
-        <v>260</v>
-      </c>
-      <c r="F35">
-        <v>91</v>
-      </c>
-      <c r="G35">
         <v>3149</v>
       </c>
     </row>

</xml_diff>